<commit_message>
Fix authentication and rename process columns
- Fixed login authentication issue preventing data editing
- Added dual authentication (Flask-Login + session)
- Enabled CORS credentials support
- Renamed process columns: 製程一/二/三/四 -> W1/W2/W3/W4
- Updated translations for W1-W4 in both Chinese and English
- Synchronized session variables on login
- Removed debug logging code
</commit_message>
<xml_diff>
--- a/鑄件盤點資料.xlsx
+++ b/鑄件盤點資料.xlsx
@@ -27057,7 +27057,7 @@
         </is>
       </c>
       <c r="C2" s="73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="123" t="n">
         <v>0</v>
@@ -27076,7 +27076,7 @@
       </c>
       <c r="I2" s="73" t="n"/>
       <c r="J2" s="83" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" s="83" t="n"/>
       <c r="L2" s="73" t="n"/>
@@ -27098,7 +27098,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="123" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="73" t="n">
         <v>0</v>
@@ -27114,7 +27114,7 @@
       </c>
       <c r="I3" s="44" t="n"/>
       <c r="J3" s="83" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K3" s="83" t="n"/>
       <c r="L3" s="44" t="n">
@@ -27180,15 +27180,18 @@
       <c r="E5" s="73" t="n">
         <v>0</v>
       </c>
-      <c r="F5" s="123" t="n"/>
-      <c r="G5" s="123" t="n"/>
+      <c r="F5" s="123" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="123" t="n">
+        <v>0</v>
+      </c>
       <c r="H5" s="73" t="n">
         <v>1</v>
       </c>
       <c r="I5" s="73" t="n"/>
-      <c r="J5" s="83">
-        <f>SUM(C5:H5)</f>
-        <v/>
+      <c r="J5" s="83" t="n">
+        <v>3</v>
       </c>
       <c r="K5" s="104" t="n"/>
       <c r="L5" s="44" t="n">

</xml_diff>